<commit_message>
Update Image Selection and Upload
</commit_message>
<xml_diff>
--- a/CredencialesRealizadas.xlsx
+++ b/CredencialesRealizadas.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:K1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,6 +489,57 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Miguel</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Angel</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Elizondo</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Herrera</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Posgrado</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>140508</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>20/03/2023</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>45371</v>
+      </c>
+      <c r="J2" t="n">
+        <v>5361564</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>C:/Users/MrJua/Desktop/SCI/Fotos/XXMKYX_00.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
UI update and Project organization
Por ahora la UI funciona en su mayoria, la segunda lista no sirve bien, ya generamos el pdf mejor y ahora solo falta voltear la pagina y arreglar ese error
</commit_message>
<xml_diff>
--- a/CredencialesRealizadas.xlsx
+++ b/CredencialesRealizadas.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:L1"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,44 +438,49 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Folio</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Nombre</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Nombre 2</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Apellido Paterno</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Apellido Materno</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Puesto</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Area</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Folio</t>
-        </is>
-      </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Registro Postgrado</t>
+          <t>Registro</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -487,6 +496,129 @@
       <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Ruta Imagen</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Encargado</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>123</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Juan</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Carlos</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Calderon</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Davila</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Director</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Directorr</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>23/03/2023</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>45374</v>
+      </c>
+      <c r="K2" t="n">
+        <v>12345</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Niels</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>C:/Users/MrJua/Downloads/20230318_002304.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Juan</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Carlos</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Calderon</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Davila</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Director</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Perro</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>23/03/2023</t>
+        </is>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>45374</v>
+      </c>
+      <c r="K3" t="n">
+        <v>165498</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Niels</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>C:/Users/MrJua/Downloads/20230318_002304.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Turn second Credential PDF page
</commit_message>
<xml_diff>
--- a/CredencialesRealizadas.xlsx
+++ b/CredencialesRealizadas.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,12 +495,12 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>Encargado</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>Ruta Imagen</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Encargado</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
         </is>
       </c>
       <c r="J2" s="2" t="n">
-        <v>45374</v>
+        <v>25568.75052516204</v>
       </c>
       <c r="K2" t="n">
         <v>12345</v>
@@ -565,10 +565,8 @@
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>123456</t>
-        </is>
+      <c r="B3" t="n">
+        <v>123456</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -606,7 +604,7 @@
         </is>
       </c>
       <c r="J3" s="2" t="n">
-        <v>45374</v>
+        <v>25568.75052516204</v>
       </c>
       <c r="K3" t="n">
         <v>165498</v>
@@ -619,6 +617,517 @@
       <c r="M3" t="inlineStr">
         <is>
           <t>C:/Users/MrJua/Downloads/20230318_002304.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="n">
+        <v>14019</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Diego</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Calderon</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Davila</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Jefe de Departamento</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Jefe de la Unidad de Informatica</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>23/03/2023</t>
+        </is>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>25568.7505250463</v>
+      </c>
+      <c r="K4" t="n">
+        <v>14253</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Niels</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>C:/Users/MrJua/Downloads/104115574_3109942045730233_5820694040960332009_n.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="n">
+        <v>156465</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Carlos</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Alberto</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Catarino</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Corralco</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Sub-director</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Subdirector Academico</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>23/03/2023</t>
+        </is>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>25568.75052494213</v>
+      </c>
+      <c r="K5" t="n">
+        <v>123123</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Niels</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>C:/Users/MrJua/Pictures/Haruu.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="n">
+        <v>123456</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Miguel</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Angel</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Elizondo</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Herrera</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Sub-director</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Subdirector Academico</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>23/03/2023</t>
+        </is>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>45374</v>
+      </c>
+      <c r="K6" t="n">
+        <v>789541</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Niels</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>C:/Users/MrJua/Desktop/SCI/Fotos/XXMKYX_00.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="n">
+        <v>456987</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Jose</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Angel</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>De la Rosa</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Aviles</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Director</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Director de la Unidad Academica</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>23/03/2023</t>
+        </is>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>45374</v>
+      </c>
+      <c r="K7" t="n">
+        <v>142537</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>C:/Users/MrJua/Downloads/Bocchi/83kcuvo4ad851.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="n">
+        <v>15014</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Roberto</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Ivan</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>De la Rosa</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Aviles</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Director</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Director de la Unidad Academica</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>23/03/2023</t>
+        </is>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>45091</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1548947</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Juan</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>C:/Users/MrJua/Downloads/Bocchi/OneDrive-2022-05-04/378.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="n">
+        <v>14018</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Juan</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Carlos</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Calderon</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Davila</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Director</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Director de la Unidad Academica</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>23/03/2023</t>
+        </is>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>45374</v>
+      </c>
+      <c r="K9" t="n">
+        <v>48456621</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Niels</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>C:/Users/MrJua/Downloads/yo.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="n">
+        <v>140198</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Juan</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Carlos</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Calderon</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Davila</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Jefe de Departamento</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Jefe de la Unidad de Informatica</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>23/03/2023</t>
+        </is>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>45374</v>
+      </c>
+      <c r="K10" t="n">
+        <v>14125574</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Niels</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>C:/Users/MrJua/Downloads/20230318_002304.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="n">
+        <v>123456</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Juan</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Carlos</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Calderon</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Davila</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Director</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Director de la Unidad Academica</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>23/03/2023</t>
+        </is>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>45374</v>
+      </c>
+      <c r="K11" t="n">
+        <v>498748</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Niels</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>C:/Users/MrJua/Downloads/Imagen de WhatsApp 2022-12-13 a las 03.15.27.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>56649874</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Jose</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Angel</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Hernandez</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Olguin</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Director</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Director de la Unidad Academica</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>23/03/2023</t>
+        </is>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>45374</v>
+      </c>
+      <c r="K12" t="n">
+        <v>140198</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Juan Carlos Calderon</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>C:/Users/MrJua/Downloads/Imagen de WhatsApp 2022-12-13 a las 03.15.27.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update de la creacion consecutiva de Credenciales
</commit_message>
<xml_diff>
--- a/CredencialesRealizadas.xlsx
+++ b/CredencialesRealizadas.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1074,10 +1074,8 @@
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>56649874</t>
-        </is>
+      <c r="B12" t="n">
+        <v>56649874</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1128,6 +1126,122 @@
       <c r="M12" t="inlineStr">
         <is>
           <t>C:/Users/MrJua/Downloads/Imagen de WhatsApp 2022-12-13 a las 03.15.27.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="n">
+        <v>140198</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Juan</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Carlos</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Calderon</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Davila</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Director</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Director de la Unidad Academica</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>23/03/2023</t>
+        </is>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>45374</v>
+      </c>
+      <c r="K13" t="n">
+        <v>141235</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Niels</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>C:/Users/MrJua/Downloads/20230318_002304.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>14019</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Juan</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Carlos</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Calderon</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Davila</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Director</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Director de la Unidad Academica</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>23/03/2023</t>
+        </is>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>45374</v>
+      </c>
+      <c r="K14" t="n">
+        <v>125465</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Niels</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>C:/Users/MrJua/Downloads/20230318_002304.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ya sirven ambos Combobox
</commit_message>
<xml_diff>
--- a/CredencialesRealizadas.xlsx
+++ b/CredencialesRealizadas.xlsx
@@ -1188,10 +1188,8 @@
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>14019</t>
-        </is>
+      <c r="B14" t="n">
+        <v>14019</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Actualizacion sobre el Nombre de los PDF
</commit_message>
<xml_diff>
--- a/CredencialesRealizadas.xlsx
+++ b/CredencialesRealizadas.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1243,6 +1243,65 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Juan</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Carlos</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Calderon</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Davila</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Sub-director</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Subdirector Administrativo</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>23/03/2023</t>
+        </is>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>45009</v>
+      </c>
+      <c r="K15" t="n">
+        <v>140198</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Niels Henrick Navarrete Manzanilla</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>C:/Users/MrJua/Downloads/20230318_002304.jpg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>